<commit_message>
Gráficos de reflectancia in situ y de las imágenes satelitales.
</commit_message>
<xml_diff>
--- a/Matchups/Datos/2019-12-10/IMG_20191210.xlsx
+++ b/Matchups/Datos/2019-12-10/IMG_20191210.xlsx
@@ -20,12 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Algoritmo</t>
+  </si>
   <si>
     <t xml:space="preserve">StationID</t>
   </si>
   <si>
+    <t xml:space="preserve">GW94-SWIR12</t>
+  </si>
+  <si>
     <t xml:space="preserve">RdP_20191210_ST06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GW94-SWIR13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GW94-SWIR23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCA-SWIR12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCA-SWIR13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCA-SWIR23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCA-SWIR123</t>
   </si>
 </sst>
 </file>
@@ -40,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,219 +164,245 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
         <v>411</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="D1" s="1" t="n">
         <v>445</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="E1" s="1" t="n">
         <v>489</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="F1" s="1" t="n">
         <v>556</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="G1" s="1" t="n">
         <v>667</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="H1" s="1" t="n">
         <v>746</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="I1" s="1" t="n">
         <v>868</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>0.0132575258612633</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>0.0259684100747108</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>0.0383884720504284</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>0.066690631210804</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>0.0645199343562126</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>0.0225970316678286</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>0.0110727716237307</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>0.0229470897465944</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>0.033242542296648</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>0.0436196736991406</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <v>0.0698573514819145</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>0.0652365237474442</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>0.0251086577773094</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>0.0129056684672833</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>0.0272510759532452</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>0.0375788398087025</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>0.0479110851883888</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="F4" s="0" t="n">
         <v>0.0739728435873985</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>0.0689310356974602</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>0.0281836781650782</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>0.0157025791704655</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="n">
         <v>0.0296916123479605</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="D5" s="0" t="n">
         <v>0.0364551581442356</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="E5" s="0" t="n">
         <v>0.0434254817664623</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <v>0.0711565539240837</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>0.0646980330348015</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>0.0210414174944162</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>0.0100848032161593</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="n">
         <v>0.434030920267105</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="E6" s="0" t="n">
         <v>0.0159025639295578</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="F6" s="0" t="n">
         <v>0.053286824375391</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>0.0595074445009232</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>0.0162639487534761</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>0.00771039817482233</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>0.0489126965403557</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="D7" s="0" t="n">
         <v>0.0505331382155419</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="E7" s="0" t="n">
         <v>0.0549294166266918</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="F7" s="0" t="n">
         <v>0.0800106078386307</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>0.0732996091246605</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>0.027456670999527</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>0.0146855106577277</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="n">
         <v>0.0405027009546757</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="D8" s="0" t="n">
         <v>0.044271495193243</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>0.0496543236076832</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="F8" s="0" t="n">
         <v>0.0743321552872658</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>0.0684394612908363</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>0.0238435119390488</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>0.0118169123306871</v>
       </c>
     </row>

</xml_diff>